<commit_message>
test adding subclasses via protege cellfie
</commit_message>
<xml_diff>
--- a/ER_CVs.xlsx
+++ b/ER_CVs.xlsx
@@ -5,17 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Library/Mobile Documents/com~apple~CloudDocs/00Work/nfdi4plants_ontology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371A82EE-D112-E146-BE11-E87FE81A51DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6CB102-7FCB-AC43-A7AD-39E8A5F9CCE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4720" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{94168D79-7187-F441-B9CC-AACC2E1AF506}"/>
   </bookViews>
   <sheets>
     <sheet name="ER CVs" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
+    <sheet name="SplitCVs" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="91">
   <si>
     <t>PROTOCOLS_library strategy</t>
   </si>
@@ -236,85 +235,160 @@
     <t>OTHER: specify</t>
   </si>
   <si>
-    <t>NFDI4PSO term label</t>
-  </si>
-  <si>
-    <t>ER term label</t>
-  </si>
-  <si>
-    <t>ER term def</t>
-  </si>
-  <si>
     <t>NFDI4PSO:0000035</t>
   </si>
   <si>
     <t>Library strategy</t>
   </si>
   <si>
-    <t>NFDI4PSO:0000036</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000037</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000038</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000039</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000040</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000041</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000042</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000043</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000044</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000045</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000046</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000047</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000048</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000049</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000050</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000051</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000052</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000053</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000054</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000055</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000056</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000057</t>
+    <t>NFDI4PSO:0000021</t>
+  </si>
+  <si>
+    <t>Raw data file format</t>
+  </si>
+  <si>
+    <t>fastq</t>
+  </si>
+  <si>
+    <t>bam</t>
+  </si>
+  <si>
+    <t>Illumina_native_qseq</t>
+  </si>
+  <si>
+    <t>Illumina_native</t>
+  </si>
+  <si>
+    <t>SOLiD_native_csfasta</t>
+  </si>
+  <si>
+    <t>SOLiD_native_qual</t>
+  </si>
+  <si>
+    <t>sff</t>
+  </si>
+  <si>
+    <t>454_native_seq</t>
+  </si>
+  <si>
+    <t>454_native_qual</t>
+  </si>
+  <si>
+    <t>Helicos_native</t>
+  </si>
+  <si>
+    <t>srf</t>
+  </si>
+  <si>
+    <t>PacBio_HDF5</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>placeholder def for RNA-Seq</t>
+  </si>
+  <si>
+    <t>placeholder def for miRNA-Seq</t>
+  </si>
+  <si>
+    <t>placeholder def for ncRNA-Seq</t>
+  </si>
+  <si>
+    <t>placeholder def for RNA-Seq (size fractionation)</t>
+  </si>
+  <si>
+    <t>placeholder def for RNA-Seq (CAGE)</t>
+  </si>
+  <si>
+    <t>placeholder def for RNA-Seq (RACE)</t>
+  </si>
+  <si>
+    <t>placeholder def for ssRNA-seq</t>
+  </si>
+  <si>
+    <t>placeholder def for ChIP-Seq</t>
+  </si>
+  <si>
+    <t>placeholder def for MNase-Seq</t>
+  </si>
+  <si>
+    <t>placeholder def for MBD-Seq</t>
+  </si>
+  <si>
+    <t>placeholder def for MRE-Seq</t>
+  </si>
+  <si>
+    <t>placeholder def for Bisulfite-Seq</t>
+  </si>
+  <si>
+    <t>placeholder def for Bisulfite-Seq (reduced representation)</t>
+  </si>
+  <si>
+    <t>placeholder def for MeDIP-Seq</t>
+  </si>
+  <si>
+    <t>placeholder def for DNase-Hypersensitivity</t>
+  </si>
+  <si>
+    <t>placeholder def for Tn-Seq</t>
+  </si>
+  <si>
+    <t>placeholder def for FAIRE-seq</t>
+  </si>
+  <si>
+    <t>placeholder def for SELEX</t>
+  </si>
+  <si>
+    <t>placeholder def for RIP-Seq</t>
+  </si>
+  <si>
+    <t>placeholder def for ATAC-seq</t>
+  </si>
+  <si>
+    <t>placeholder def for ChIA-PET</t>
+  </si>
+  <si>
+    <t>placeholder def for Hi-C</t>
+  </si>
+  <si>
+    <t>placeholder def for OTHER: specify</t>
+  </si>
+  <si>
+    <t>placeholder def for fastq</t>
+  </si>
+  <si>
+    <t>placeholder def for bam</t>
+  </si>
+  <si>
+    <t>placeholder def for Illumina_native_qseq</t>
+  </si>
+  <si>
+    <t>placeholder def for Illumina_native</t>
+  </si>
+  <si>
+    <t>placeholder def for SOLiD_native_csfasta</t>
+  </si>
+  <si>
+    <t>placeholder def for SOLiD_native_qual</t>
+  </si>
+  <si>
+    <t>placeholder def for sff</t>
+  </si>
+  <si>
+    <t>placeholder def for 454_native_seq</t>
+  </si>
+  <si>
+    <t>placeholder def for 454_native_qual</t>
+  </si>
+  <si>
+    <t>placeholder def for Helicos_native</t>
+  </si>
+  <si>
+    <t>placeholder def for srf</t>
+  </si>
+  <si>
+    <t>placeholder def for PacBio_HDF5</t>
   </si>
 </sst>
 </file>
@@ -344,7 +418,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,14 +431,8 @@
         <bgColor theme="4"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -386,11 +454,20 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color theme="4" tint="0.39997558519241921"/>
       </bottom>
@@ -401,9 +478,7 @@
       <right style="thin">
         <color theme="4" tint="0.39997558519241921"/>
       </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color theme="4" tint="0.39997558519241921"/>
       </bottom>
@@ -413,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -421,29 +496,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -468,89 +543,19 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
-        <top/>
-        <bottom/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
+      <border outline="0">
         <top style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -588,31 +593,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6AACB006-DD01-D04A-B78C-EBDBAE76FD63}" name="Table1" displayName="Table1" ref="A1:E7" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6AACB006-DD01-D04A-B78C-EBDBAE76FD63}" name="Table1" displayName="Table1" ref="A1:E7" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:E7" xr:uid="{6AACB006-DD01-D04A-B78C-EBDBAE76FD63}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{BA3FF105-7952-124F-A428-EC8FB3C5D362}" name="NFDI4PSO term id" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{DA1360EC-3F6F-1849-B5E2-909A53BBD1AB}" name="NFDI4PSO term name" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{5EF530B9-0648-7941-B24A-8736A9BE1385}" name="ER" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{60426845-DBE8-A649-A831-E3BBB6BA9EA7}" name="ER target" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{74A2C2D1-CEE5-1D42-82B5-38002B29C965}" name="ER required cv" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{BA3FF105-7952-124F-A428-EC8FB3C5D362}" name="NFDI4PSO term id" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{DA1360EC-3F6F-1849-B5E2-909A53BBD1AB}" name="NFDI4PSO term name" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{5EF530B9-0648-7941-B24A-8736A9BE1385}" name="ER" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{60426845-DBE8-A649-A831-E3BBB6BA9EA7}" name="ER target" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{74A2C2D1-CEE5-1D42-82B5-38002B29C965}" name="ER required cv" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6CB6C22D-0845-6445-8713-6125F4B09DF4}" name="Table2" displayName="Table2" ref="A1:F24" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:F24" xr:uid="{6CB6C22D-0845-6445-8713-6125F4B09DF4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{89A4AE18-6C4A-CB4C-A3BA-E333F5C3FF45}" name="Table2" displayName="Table2" ref="A1:F36" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="2" tableBorderDxfId="3">
+  <autoFilter ref="A1:F36" xr:uid="{89A4AE18-6C4A-CB4C-A3BA-E333F5C3FF45}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{5C680FB0-1BA9-6442-B1AF-76863C0AD79F}" name="NFDI4PSO term id"/>
-    <tableColumn id="2" xr3:uid="{37A5855C-C7CE-DC4B-89B3-9EA3659D2126}" name="NFDI4PSO term label"/>
-    <tableColumn id="3" xr3:uid="{45DB3ECA-0E62-0B4D-9F1F-39F33F2D2FC3}" name="ER" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{B7BAC418-345C-5044-8759-C716106BAE32}" name="ER target" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{DD662029-2AD4-DD4A-9FFA-AA6F60B75001}" name="ER term label"/>
-    <tableColumn id="7" xr3:uid="{74FF63AA-742D-2A4F-BD27-2603C13F8E71}" name="ER term def">
-      <calculatedColumnFormula>CONCATENATE("placeholder def of ", E2)</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="1" xr3:uid="{8A758B73-37C9-674C-AF03-DC7147CC6A13}" name="NFDI4PSO term id"/>
+    <tableColumn id="2" xr3:uid="{A623808C-31DE-E449-B98F-F28273B5AA4C}" name="NFDI4PSO term name"/>
+    <tableColumn id="3" xr3:uid="{052A2D10-C22E-7F4D-B2C4-F68DB511BDB8}" name="ER"/>
+    <tableColumn id="4" xr3:uid="{576548E7-AD3A-9945-8A8E-92C64E5F99AF}" name="ER target"/>
+    <tableColumn id="5" xr3:uid="{5C5241C0-93A6-6543-9ADC-3802A375B964}" name="ER required cv"/>
+    <tableColumn id="6" xr3:uid="{590546A3-A484-E74A-A424-E2AC5B610D01}" name="def" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -917,16 +920,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5962EDB-2ADA-344C-BBAD-104050921182}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="67" workbookViewId="0">
-      <selection activeCell="E2" sqref="A1:E2"/>
+    <sheetView zoomScale="89" workbookViewId="0">
+      <selection activeCell="E3" sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
-    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34" customWidth="1"/>
     <col min="5" max="5" width="52.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -948,8 +951,12 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="404" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
@@ -961,8 +968,12 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="238" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
@@ -1031,524 +1042,740 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871F3FA3-5F76-2B44-8BD0-23BD925CC6D1}">
-  <dimension ref="A1:F24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4367F48-ECBC-E941-A5EF-8D3208BCE9E8}">
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="E10" sqref="E10:E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.83203125" customWidth="1"/>
-    <col min="2" max="2" width="26.83203125" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" customWidth="1"/>
-    <col min="4" max="4" width="28.83203125" customWidth="1"/>
-    <col min="5" max="5" width="33.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="38.33203125" customWidth="1"/>
+    <col min="5" max="6" width="33.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>41</v>
+      <c r="E1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="str">
-        <f>CONCATENATE("placeholder def of ", E2)</f>
-        <v>placeholder def of RNA-Seq</v>
+      <c r="F2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
         <v>0</v>
       </c>
       <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="str">
-        <f t="shared" ref="F3:F24" si="0">CONCATENATE("placeholder def of ", E3)</f>
-        <v>placeholder def of miRNA-Seq</v>
+      <c r="F3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="s">
         <v>18</v>
       </c>
-      <c r="F4" t="str">
-        <f t="shared" si="0"/>
-        <v>placeholder def of ncRNA-Seq</v>
+      <c r="F4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
         <v>0</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="F5" t="str">
-        <f t="shared" si="0"/>
-        <v>placeholder def of RNA-Seq (size fractionation)</v>
+      <c r="F5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
         <v>0</v>
       </c>
       <c r="E6" t="s">
         <v>20</v>
       </c>
-      <c r="F6" t="str">
-        <f t="shared" si="0"/>
-        <v>placeholder def of RNA-Seq (CAGE)</v>
+      <c r="F6" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
         <v>0</v>
       </c>
       <c r="E7" t="s">
         <v>21</v>
       </c>
-      <c r="F7" t="str">
-        <f t="shared" si="0"/>
-        <v>placeholder def of RNA-Seq (RACE)</v>
+      <c r="F7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
         <v>0</v>
       </c>
       <c r="E8" t="s">
         <v>22</v>
       </c>
-      <c r="F8" t="str">
-        <f t="shared" si="0"/>
-        <v>placeholder def of ssRNA-seq</v>
+      <c r="F8" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
         <v>0</v>
       </c>
       <c r="E9" t="s">
         <v>23</v>
       </c>
-      <c r="F9" t="str">
-        <f t="shared" si="0"/>
-        <v>placeholder def of ChIP-Seq</v>
+      <c r="F9" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
         <v>0</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
       </c>
-      <c r="F10" t="str">
-        <f t="shared" si="0"/>
-        <v>placeholder def of MNase-Seq</v>
+      <c r="F10" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
         <v>0</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
       </c>
-      <c r="F11" t="str">
-        <f t="shared" si="0"/>
-        <v>placeholder def of MBD-Seq</v>
+      <c r="F11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
         <v>0</v>
       </c>
       <c r="E12" t="s">
         <v>26</v>
       </c>
-      <c r="F12" t="str">
-        <f t="shared" si="0"/>
-        <v>placeholder def of MRE-Seq</v>
+      <c r="F12" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
         <v>0</v>
       </c>
       <c r="E13" t="s">
         <v>27</v>
       </c>
-      <c r="F13" t="str">
-        <f t="shared" si="0"/>
-        <v>placeholder def of Bisulfite-Seq</v>
+      <c r="F13" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
         <v>0</v>
       </c>
       <c r="E14" t="s">
         <v>28</v>
       </c>
-      <c r="F14" t="str">
-        <f t="shared" si="0"/>
-        <v>placeholder def of Bisulfite-Seq (reduced representation)</v>
+      <c r="F14" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
         <v>0</v>
       </c>
       <c r="E15" t="s">
         <v>29</v>
       </c>
-      <c r="F15" t="str">
-        <f t="shared" si="0"/>
-        <v>placeholder def of MeDIP-Seq</v>
+      <c r="F15" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
         <v>0</v>
       </c>
       <c r="E16" t="s">
         <v>30</v>
       </c>
-      <c r="F16" t="str">
-        <f t="shared" si="0"/>
-        <v>placeholder def of DNase-Hypersensitivity</v>
+      <c r="F16" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
         <v>0</v>
       </c>
       <c r="E17" t="s">
         <v>31</v>
       </c>
-      <c r="F17" t="str">
-        <f t="shared" si="0"/>
-        <v>placeholder def of Tn-Seq</v>
+      <c r="F17" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
         <v>0</v>
       </c>
       <c r="E18" t="s">
         <v>32</v>
       </c>
-      <c r="F18" t="str">
-        <f t="shared" si="0"/>
-        <v>placeholder def of FAIRE-seq</v>
+      <c r="F18" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
         <v>0</v>
       </c>
       <c r="E19" t="s">
         <v>33</v>
       </c>
-      <c r="F19" t="str">
-        <f t="shared" si="0"/>
-        <v>placeholder def of SELEX</v>
+      <c r="F19" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
         <v>0</v>
       </c>
       <c r="E20" t="s">
         <v>34</v>
       </c>
-      <c r="F20" t="str">
-        <f t="shared" si="0"/>
-        <v>placeholder def of RIP-Seq</v>
+      <c r="F20" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s">
         <v>0</v>
       </c>
       <c r="E21" t="s">
         <v>35</v>
       </c>
-      <c r="F21" t="str">
-        <f t="shared" si="0"/>
-        <v>placeholder def of ATAC-seq</v>
+      <c r="F21" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s">
         <v>0</v>
       </c>
       <c r="E22" t="s">
         <v>36</v>
       </c>
-      <c r="F22" t="str">
-        <f t="shared" si="0"/>
-        <v>placeholder def of ChIA-PET</v>
+      <c r="F22" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" t="s">
         <v>0</v>
       </c>
       <c r="E23" t="s">
         <v>37</v>
       </c>
-      <c r="F23" t="str">
-        <f t="shared" si="0"/>
-        <v>placeholder def of Hi-C</v>
+      <c r="F23" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" t="s">
         <v>0</v>
       </c>
       <c r="E24" t="s">
         <v>38</v>
       </c>
-      <c r="F24" t="str">
-        <f t="shared" si="0"/>
-        <v>placeholder def of OTHER: specify</v>
+      <c r="F24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>49</v>
+      </c>
+      <c r="F31" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>50</v>
+      </c>
+      <c r="F32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>51</v>
+      </c>
+      <c r="F33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>52</v>
+      </c>
+      <c r="F34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>54</v>
+      </c>
+      <c r="F36" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1558,35 +1785,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5BAD436-BA9C-0B4F-8B2B-99D7FB58FEEA}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="5" max="5" width="33.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="404" x14ac:dyDescent="0.2">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
more GEO required cv
</commit_message>
<xml_diff>
--- a/ER_CVs.xlsx
+++ b/ER_CVs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Library/Mobile Documents/com~apple~CloudDocs/00Work/nfdi4plants_ontology/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F286508-EF5E-054E-8F39-0022055DCBBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFDB599-964C-9B43-815E-1051150E2B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1320" yWindow="-21100" windowWidth="29300" windowHeight="21100" activeTab="1" xr2:uid="{94168D79-7187-F441-B9CC-AACC2E1AF506}"/>
+    <workbookView xWindow="10140" yWindow="-21100" windowWidth="22860" windowHeight="21100" activeTab="1" xr2:uid="{94168D79-7187-F441-B9CC-AACC2E1AF506}"/>
   </bookViews>
   <sheets>
     <sheet name="ER CVs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="211">
   <si>
     <t>PROTOCOLS_library strategy</t>
   </si>
@@ -286,109 +286,469 @@
     <t>def</t>
   </si>
   <si>
-    <t>placeholder def ofRNA-Seq</t>
-  </si>
-  <si>
-    <t>placeholder def ofmiRNA-Seq</t>
-  </si>
-  <si>
-    <t>placeholder def ofncRNA-Seq</t>
-  </si>
-  <si>
-    <t>placeholder def ofRNA-Seq (size fractionation)</t>
-  </si>
-  <si>
-    <t>placeholder def ofRNA-Seq (CAGE)</t>
-  </si>
-  <si>
-    <t>placeholder def ofRNA-Seq (RACE)</t>
-  </si>
-  <si>
-    <t>placeholder def ofssRNA-seq</t>
-  </si>
-  <si>
-    <t>placeholder def ofChIP-Seq</t>
-  </si>
-  <si>
-    <t>placeholder def ofMNase-Seq</t>
-  </si>
-  <si>
-    <t>placeholder def ofMBD-Seq</t>
-  </si>
-  <si>
-    <t>placeholder def ofMRE-Seq</t>
-  </si>
-  <si>
-    <t>placeholder def ofBisulfite-Seq</t>
-  </si>
-  <si>
-    <t>placeholder def ofBisulfite-Seq (reduced representation)</t>
-  </si>
-  <si>
-    <t>placeholder def ofMeDIP-Seq</t>
-  </si>
-  <si>
-    <t>placeholder def ofDNase-Hypersensitivity</t>
-  </si>
-  <si>
-    <t>placeholder def ofTn-Seq</t>
-  </si>
-  <si>
-    <t>placeholder def ofFAIRE-seq</t>
-  </si>
-  <si>
-    <t>placeholder def ofSELEX</t>
-  </si>
-  <si>
-    <t>placeholder def ofRIP-Seq</t>
-  </si>
-  <si>
-    <t>placeholder def ofATAC-seq</t>
-  </si>
-  <si>
-    <t>placeholder def ofChIA-PET</t>
-  </si>
-  <si>
-    <t>placeholder def ofHi-C</t>
-  </si>
-  <si>
-    <t>placeholder def ofOTHER: specify</t>
-  </si>
-  <si>
-    <t>placeholder def offastq</t>
-  </si>
-  <si>
-    <t>placeholder def ofbam</t>
-  </si>
-  <si>
-    <t>placeholder def ofIllumina_native_qseq</t>
-  </si>
-  <si>
-    <t>placeholder def ofIllumina_native</t>
-  </si>
-  <si>
-    <t>placeholder def ofSOLiD_native_csfasta</t>
-  </si>
-  <si>
-    <t>placeholder def ofSOLiD_native_qual</t>
-  </si>
-  <si>
-    <t>placeholder def ofsff</t>
-  </si>
-  <si>
-    <t>placeholder def of454_native_seq</t>
-  </si>
-  <si>
-    <t>placeholder def of454_native_qual</t>
-  </si>
-  <si>
-    <t>placeholder def ofHelicos_native</t>
-  </si>
-  <si>
-    <t>placeholder def ofsrf</t>
-  </si>
-  <si>
-    <t>placeholder def ofPacBio_HDF5</t>
+    <t>Illumina Genome Analyzer IIx</t>
+  </si>
+  <si>
+    <t>Illumina HiSeq 1000</t>
+  </si>
+  <si>
+    <t>Illumina HiSeq 1500</t>
+  </si>
+  <si>
+    <t>Illumina HiSeq 2000</t>
+  </si>
+  <si>
+    <t>Illumina HiSeq 2500</t>
+  </si>
+  <si>
+    <t>Illumina HiSeq 3000</t>
+  </si>
+  <si>
+    <t>Illumina HiSeq 4000</t>
+  </si>
+  <si>
+    <t>Illumina NextSeq 500</t>
+  </si>
+  <si>
+    <t>Illumina NextSeq 550</t>
+  </si>
+  <si>
+    <t>Illumina HiSeq X Ten</t>
+  </si>
+  <si>
+    <t>Illumina HiSeq X Five</t>
+  </si>
+  <si>
+    <t>Illumina NovaSeq 6000</t>
+  </si>
+  <si>
+    <t>Illumina MiSeq</t>
+  </si>
+  <si>
+    <t>Illumina HiScanSQ</t>
+  </si>
+  <si>
+    <t>Illumina MiniSeq</t>
+  </si>
+  <si>
+    <t>Illumina iSeq 100</t>
+  </si>
+  <si>
+    <t>BGISEQ-500</t>
+  </si>
+  <si>
+    <t>DNBSEQ-G400</t>
+  </si>
+  <si>
+    <t>DNBSEQ-T7</t>
+  </si>
+  <si>
+    <t>DNBSEQ-G50</t>
+  </si>
+  <si>
+    <t>Ion Torrent PGM</t>
+  </si>
+  <si>
+    <t>Ion Torrent Proton</t>
+  </si>
+  <si>
+    <t>Ion Torrent S5</t>
+  </si>
+  <si>
+    <t>Ion Torrent S5 XL</t>
+  </si>
+  <si>
+    <t>PacBio RS</t>
+  </si>
+  <si>
+    <t>PacBio RS II</t>
+  </si>
+  <si>
+    <t>Sequel</t>
+  </si>
+  <si>
+    <t>Sequel II</t>
+  </si>
+  <si>
+    <t>AB SOLiD System 2.0</t>
+  </si>
+  <si>
+    <t>AB SOLiD System 3.0</t>
+  </si>
+  <si>
+    <t>AB SOLiD 3 Plus System</t>
+  </si>
+  <si>
+    <t>AB SOLiD 4 System</t>
+  </si>
+  <si>
+    <t>AB SOLiD 4hq System</t>
+  </si>
+  <si>
+    <t>AB SOLiD PI System</t>
+  </si>
+  <si>
+    <t>AB 5500 Genetic Analyzer</t>
+  </si>
+  <si>
+    <t>AB 5500xl Genetic Analyzer</t>
+  </si>
+  <si>
+    <t>AB 5500xl-W Genetic Analysis System</t>
+  </si>
+  <si>
+    <t>454 GS</t>
+  </si>
+  <si>
+    <t>454 GS 20</t>
+  </si>
+  <si>
+    <t>454 GS FLX</t>
+  </si>
+  <si>
+    <t>454 GS FLX+</t>
+  </si>
+  <si>
+    <t>454 GS Junior</t>
+  </si>
+  <si>
+    <t>454 GS FLX Titanium</t>
+  </si>
+  <si>
+    <t>Complete Genomics</t>
+  </si>
+  <si>
+    <t>Helicos HeliScope</t>
+  </si>
+  <si>
+    <t>GridION</t>
+  </si>
+  <si>
+    <t>MinION</t>
+  </si>
+  <si>
+    <t>PromethION</t>
+  </si>
+  <si>
+    <t>single</t>
+  </si>
+  <si>
+    <t>paired-end</t>
+  </si>
+  <si>
+    <t>total RNA</t>
+  </si>
+  <si>
+    <t>polyA RNA</t>
+  </si>
+  <si>
+    <t>cytoplasmic RNA</t>
+  </si>
+  <si>
+    <t>nuclear RNA</t>
+  </si>
+  <si>
+    <t>genomic DNA</t>
+  </si>
+  <si>
+    <t>protein</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>placeholder def of RNA-Seq</t>
+  </si>
+  <si>
+    <t>placeholder def of miRNA-Seq</t>
+  </si>
+  <si>
+    <t>placeholder def of ncRNA-Seq</t>
+  </si>
+  <si>
+    <t>placeholder def of RNA-Seq (size fractionation)</t>
+  </si>
+  <si>
+    <t>placeholder def of RNA-Seq (CAGE)</t>
+  </si>
+  <si>
+    <t>placeholder def of RNA-Seq (RACE)</t>
+  </si>
+  <si>
+    <t>placeholder def of ssRNA-seq</t>
+  </si>
+  <si>
+    <t>placeholder def of ChIP-Seq</t>
+  </si>
+  <si>
+    <t>placeholder def of MNase-Seq</t>
+  </si>
+  <si>
+    <t>placeholder def of MBD-Seq</t>
+  </si>
+  <si>
+    <t>placeholder def of MRE-Seq</t>
+  </si>
+  <si>
+    <t>placeholder def of Bisulfite-Seq</t>
+  </si>
+  <si>
+    <t>placeholder def of Bisulfite-Seq (reduced representation)</t>
+  </si>
+  <si>
+    <t>placeholder def of MeDIP-Seq</t>
+  </si>
+  <si>
+    <t>placeholder def of DNase-Hypersensitivity</t>
+  </si>
+  <si>
+    <t>placeholder def of Tn-Seq</t>
+  </si>
+  <si>
+    <t>placeholder def of FAIRE-seq</t>
+  </si>
+  <si>
+    <t>placeholder def of SELEX</t>
+  </si>
+  <si>
+    <t>placeholder def of RIP-Seq</t>
+  </si>
+  <si>
+    <t>placeholder def of ATAC-seq</t>
+  </si>
+  <si>
+    <t>placeholder def of ChIA-PET</t>
+  </si>
+  <si>
+    <t>placeholder def of Hi-C</t>
+  </si>
+  <si>
+    <t>placeholder def of OTHER: specify</t>
+  </si>
+  <si>
+    <t>placeholder def of fastq</t>
+  </si>
+  <si>
+    <t>placeholder def of bam</t>
+  </si>
+  <si>
+    <t>placeholder def of Illumina_native_qseq</t>
+  </si>
+  <si>
+    <t>placeholder def of Illumina_native</t>
+  </si>
+  <si>
+    <t>placeholder def of SOLiD_native_csfasta</t>
+  </si>
+  <si>
+    <t>placeholder def of SOLiD_native_qual</t>
+  </si>
+  <si>
+    <t>placeholder def of sff</t>
+  </si>
+  <si>
+    <t>placeholder def of 454_native_seq</t>
+  </si>
+  <si>
+    <t>placeholder def of 454_native_qual</t>
+  </si>
+  <si>
+    <t>placeholder def of Helicos_native</t>
+  </si>
+  <si>
+    <t>placeholder def of srf</t>
+  </si>
+  <si>
+    <t>placeholder def of PacBio_HDF5</t>
+  </si>
+  <si>
+    <t>placeholder def of Illumina Genome Analyzer IIx</t>
+  </si>
+  <si>
+    <t>placeholder def of Illumina HiSeq 1000</t>
+  </si>
+  <si>
+    <t>placeholder def of Illumina HiSeq 1500</t>
+  </si>
+  <si>
+    <t>placeholder def of Illumina HiSeq 2000</t>
+  </si>
+  <si>
+    <t>placeholder def of Illumina HiSeq 2500</t>
+  </si>
+  <si>
+    <t>placeholder def of Illumina HiSeq 3000</t>
+  </si>
+  <si>
+    <t>placeholder def of Illumina HiSeq 4000</t>
+  </si>
+  <si>
+    <t>placeholder def of Illumina NextSeq 500</t>
+  </si>
+  <si>
+    <t>placeholder def of Illumina NextSeq 550</t>
+  </si>
+  <si>
+    <t>placeholder def of Illumina HiSeq X Ten</t>
+  </si>
+  <si>
+    <t>placeholder def of Illumina HiSeq X Five</t>
+  </si>
+  <si>
+    <t>placeholder def of Illumina NovaSeq 6000</t>
+  </si>
+  <si>
+    <t>placeholder def of Illumina MiSeq</t>
+  </si>
+  <si>
+    <t>placeholder def of Illumina HiScanSQ</t>
+  </si>
+  <si>
+    <t>placeholder def of Illumina MiniSeq</t>
+  </si>
+  <si>
+    <t>placeholder def of Illumina iSeq 100</t>
+  </si>
+  <si>
+    <t>placeholder def of BGISEQ-500</t>
+  </si>
+  <si>
+    <t>placeholder def of DNBSEQ-G400</t>
+  </si>
+  <si>
+    <t>placeholder def of DNBSEQ-T7</t>
+  </si>
+  <si>
+    <t>placeholder def of DNBSEQ-G50</t>
+  </si>
+  <si>
+    <t>placeholder def of Ion Torrent PGM</t>
+  </si>
+  <si>
+    <t>placeholder def of Ion Torrent Proton</t>
+  </si>
+  <si>
+    <t>placeholder def of Ion Torrent S5</t>
+  </si>
+  <si>
+    <t>placeholder def of Ion Torrent S5 XL</t>
+  </si>
+  <si>
+    <t>placeholder def of PacBio RS</t>
+  </si>
+  <si>
+    <t>placeholder def of PacBio RS II</t>
+  </si>
+  <si>
+    <t>placeholder def of Sequel</t>
+  </si>
+  <si>
+    <t>placeholder def of Sequel II</t>
+  </si>
+  <si>
+    <t>placeholder def of AB SOLiD System 2.0</t>
+  </si>
+  <si>
+    <t>placeholder def of AB SOLiD System 3.0</t>
+  </si>
+  <si>
+    <t>placeholder def of AB SOLiD 3 Plus System</t>
+  </si>
+  <si>
+    <t>placeholder def of AB SOLiD 4 System</t>
+  </si>
+  <si>
+    <t>placeholder def of AB SOLiD 4hq System</t>
+  </si>
+  <si>
+    <t>placeholder def of AB SOLiD PI System</t>
+  </si>
+  <si>
+    <t>placeholder def of AB 5500 Genetic Analyzer</t>
+  </si>
+  <si>
+    <t>placeholder def of AB 5500xl Genetic Analyzer</t>
+  </si>
+  <si>
+    <t>placeholder def of AB 5500xl-W Genetic Analysis System</t>
+  </si>
+  <si>
+    <t>placeholder def of 454 GS</t>
+  </si>
+  <si>
+    <t>placeholder def of 454 GS 20</t>
+  </si>
+  <si>
+    <t>placeholder def of 454 GS FLX</t>
+  </si>
+  <si>
+    <t>placeholder def of 454 GS FLX+</t>
+  </si>
+  <si>
+    <t>placeholder def of 454 GS Junior</t>
+  </si>
+  <si>
+    <t>placeholder def of 454 GS FLX Titanium</t>
+  </si>
+  <si>
+    <t>placeholder def of Complete Genomics</t>
+  </si>
+  <si>
+    <t>placeholder def of Helicos HeliScope</t>
+  </si>
+  <si>
+    <t>placeholder def of GridION</t>
+  </si>
+  <si>
+    <t>placeholder def of MinION</t>
+  </si>
+  <si>
+    <t>placeholder def of PromethION</t>
+  </si>
+  <si>
+    <t>placeholder def of single</t>
+  </si>
+  <si>
+    <t>placeholder def of paired-end</t>
+  </si>
+  <si>
+    <t>placeholder def of total RNA</t>
+  </si>
+  <si>
+    <t>placeholder def of polyA RNA</t>
+  </si>
+  <si>
+    <t>placeholder def of cytoplasmic RNA</t>
+  </si>
+  <si>
+    <t>placeholder def of nuclear RNA</t>
+  </si>
+  <si>
+    <t>placeholder def of genomic DNA</t>
+  </si>
+  <si>
+    <t>placeholder def of protein</t>
+  </si>
+  <si>
+    <t>placeholder def of other</t>
+  </si>
+  <si>
+    <t>Next generation sequencing instrument model</t>
+  </si>
+  <si>
+    <t>NFDI4PSO:0000040</t>
+  </si>
+  <si>
+    <t>Bio entity</t>
+  </si>
+  <si>
+    <t>NFDI4PSO:0000012</t>
+  </si>
+  <si>
+    <t>Library layout</t>
+  </si>
+  <si>
+    <t>NFDI4PSO:0000015</t>
   </si>
 </sst>
 </file>
@@ -809,8 +1169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5962EDB-2ADA-344C-BBAD-104050921182}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="A1:E3"/>
+    <sheetView topLeftCell="A3" zoomScale="75" workbookViewId="0">
+      <selection activeCell="E7" sqref="A4:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -932,16 +1292,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9663FC99-9848-9249-B432-18F617F0549A}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="75" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="33.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+    <col min="2" max="2" width="53.1640625" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="35.83203125" customWidth="1"/>
+    <col min="5" max="5" width="42.5" customWidth="1"/>
+    <col min="6" max="6" width="62.5" customWidth="1"/>
+    <col min="7" max="7" width="52" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -981,7 +1346,7 @@
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1001,7 +1366,7 @@
         <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1021,7 +1386,7 @@
         <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1041,7 +1406,7 @@
         <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1061,7 +1426,7 @@
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>60</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1081,7 +1446,7 @@
         <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1101,7 +1466,7 @@
         <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>62</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1121,7 +1486,7 @@
         <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>63</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1141,7 +1506,7 @@
         <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>64</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1161,7 +1526,7 @@
         <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1181,7 +1546,7 @@
         <v>26</v>
       </c>
       <c r="F12" t="s">
-        <v>66</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1201,7 +1566,7 @@
         <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>67</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1221,7 +1586,7 @@
         <v>28</v>
       </c>
       <c r="F14" t="s">
-        <v>68</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1241,7 +1606,7 @@
         <v>29</v>
       </c>
       <c r="F15" t="s">
-        <v>69</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1261,7 +1626,7 @@
         <v>30</v>
       </c>
       <c r="F16" t="s">
-        <v>70</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1281,7 +1646,7 @@
         <v>31</v>
       </c>
       <c r="F17" t="s">
-        <v>71</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1301,7 +1666,7 @@
         <v>32</v>
       </c>
       <c r="F18" t="s">
-        <v>72</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1321,7 +1686,7 @@
         <v>33</v>
       </c>
       <c r="F19" t="s">
-        <v>73</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1341,7 +1706,7 @@
         <v>34</v>
       </c>
       <c r="F20" t="s">
-        <v>74</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1361,7 +1726,7 @@
         <v>35</v>
       </c>
       <c r="F21" t="s">
-        <v>75</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1381,7 +1746,7 @@
         <v>36</v>
       </c>
       <c r="F22" t="s">
-        <v>76</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1401,7 +1766,7 @@
         <v>37</v>
       </c>
       <c r="F23" t="s">
-        <v>77</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1421,7 +1786,7 @@
         <v>38</v>
       </c>
       <c r="F24" t="s">
-        <v>78</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1441,7 +1806,7 @@
         <v>43</v>
       </c>
       <c r="F25" t="s">
-        <v>79</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1461,7 +1826,7 @@
         <v>44</v>
       </c>
       <c r="F26" t="s">
-        <v>80</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1481,7 +1846,7 @@
         <v>45</v>
       </c>
       <c r="F27" t="s">
-        <v>81</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1501,7 +1866,7 @@
         <v>46</v>
       </c>
       <c r="F28" t="s">
-        <v>82</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1521,7 +1886,7 @@
         <v>47</v>
       </c>
       <c r="F29" t="s">
-        <v>83</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1541,7 +1906,7 @@
         <v>48</v>
       </c>
       <c r="F30" t="s">
-        <v>84</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1561,7 +1926,7 @@
         <v>49</v>
       </c>
       <c r="F31" t="s">
-        <v>85</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1581,7 +1946,7 @@
         <v>50</v>
       </c>
       <c r="F32" t="s">
-        <v>86</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1601,7 +1966,7 @@
         <v>51</v>
       </c>
       <c r="F33" t="s">
-        <v>87</v>
+        <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1621,7 +1986,7 @@
         <v>52</v>
       </c>
       <c r="F34" t="s">
-        <v>88</v>
+        <v>145</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1641,7 +2006,7 @@
         <v>53</v>
       </c>
       <c r="F35" t="s">
-        <v>89</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1661,7 +2026,1147 @@
         <v>54</v>
       </c>
       <c r="F36" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>206</v>
+      </c>
+      <c r="B37" t="s">
+        <v>205</v>
+      </c>
+      <c r="C37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>56</v>
+      </c>
+      <c r="F37" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>206</v>
+      </c>
+      <c r="B38" t="s">
+        <v>205</v>
+      </c>
+      <c r="C38" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38" t="s">
+        <v>57</v>
+      </c>
+      <c r="F38" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>206</v>
+      </c>
+      <c r="B39" t="s">
+        <v>205</v>
+      </c>
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" t="s">
+        <v>2</v>
+      </c>
+      <c r="E39" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>206</v>
+      </c>
+      <c r="B40" t="s">
+        <v>205</v>
+      </c>
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" t="s">
+        <v>59</v>
+      </c>
+      <c r="F40" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>206</v>
+      </c>
+      <c r="B41" t="s">
+        <v>205</v>
+      </c>
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" t="s">
+        <v>2</v>
+      </c>
+      <c r="E41" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>206</v>
+      </c>
+      <c r="B42" t="s">
+        <v>205</v>
+      </c>
+      <c r="C42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>206</v>
+      </c>
+      <c r="B43" t="s">
+        <v>205</v>
+      </c>
+      <c r="C43" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" t="s">
+        <v>2</v>
+      </c>
+      <c r="E43" t="s">
+        <v>62</v>
+      </c>
+      <c r="F43" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>206</v>
+      </c>
+      <c r="B44" t="s">
+        <v>205</v>
+      </c>
+      <c r="C44" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" t="s">
+        <v>2</v>
+      </c>
+      <c r="E44" t="s">
+        <v>63</v>
+      </c>
+      <c r="F44" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>206</v>
+      </c>
+      <c r="B45" t="s">
+        <v>205</v>
+      </c>
+      <c r="C45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" t="s">
+        <v>64</v>
+      </c>
+      <c r="F45" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>206</v>
+      </c>
+      <c r="B46" t="s">
+        <v>205</v>
+      </c>
+      <c r="C46" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" t="s">
+        <v>2</v>
+      </c>
+      <c r="E46" t="s">
+        <v>65</v>
+      </c>
+      <c r="F46" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>206</v>
+      </c>
+      <c r="B47" t="s">
+        <v>205</v>
+      </c>
+      <c r="C47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" t="s">
+        <v>2</v>
+      </c>
+      <c r="E47" t="s">
+        <v>66</v>
+      </c>
+      <c r="F47" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>206</v>
+      </c>
+      <c r="B48" t="s">
+        <v>205</v>
+      </c>
+      <c r="C48" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" t="s">
+        <v>2</v>
+      </c>
+      <c r="E48" t="s">
+        <v>67</v>
+      </c>
+      <c r="F48" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>206</v>
+      </c>
+      <c r="B49" t="s">
+        <v>205</v>
+      </c>
+      <c r="C49" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" t="s">
+        <v>68</v>
+      </c>
+      <c r="F49" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>206</v>
+      </c>
+      <c r="B50" t="s">
+        <v>205</v>
+      </c>
+      <c r="C50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" t="s">
+        <v>2</v>
+      </c>
+      <c r="E50" t="s">
+        <v>69</v>
+      </c>
+      <c r="F50" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>206</v>
+      </c>
+      <c r="B51" t="s">
+        <v>205</v>
+      </c>
+      <c r="C51" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" t="s">
+        <v>2</v>
+      </c>
+      <c r="E51" t="s">
+        <v>70</v>
+      </c>
+      <c r="F51" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>206</v>
+      </c>
+      <c r="B52" t="s">
+        <v>205</v>
+      </c>
+      <c r="C52" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" t="s">
+        <v>2</v>
+      </c>
+      <c r="E52" t="s">
+        <v>71</v>
+      </c>
+      <c r="F52" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>206</v>
+      </c>
+      <c r="B53" t="s">
+        <v>205</v>
+      </c>
+      <c r="C53" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" t="s">
+        <v>2</v>
+      </c>
+      <c r="E53" t="s">
+        <v>72</v>
+      </c>
+      <c r="F53" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>206</v>
+      </c>
+      <c r="B54" t="s">
+        <v>205</v>
+      </c>
+      <c r="C54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" t="s">
+        <v>2</v>
+      </c>
+      <c r="E54" t="s">
+        <v>73</v>
+      </c>
+      <c r="F54" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>206</v>
+      </c>
+      <c r="B55" t="s">
+        <v>205</v>
+      </c>
+      <c r="C55" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" t="s">
+        <v>2</v>
+      </c>
+      <c r="E55" t="s">
+        <v>74</v>
+      </c>
+      <c r="F55" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>206</v>
+      </c>
+      <c r="B56" t="s">
+        <v>205</v>
+      </c>
+      <c r="C56" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" t="s">
+        <v>2</v>
+      </c>
+      <c r="E56" t="s">
+        <v>75</v>
+      </c>
+      <c r="F56" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>206</v>
+      </c>
+      <c r="B57" t="s">
+        <v>205</v>
+      </c>
+      <c r="C57" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" t="s">
+        <v>2</v>
+      </c>
+      <c r="E57" t="s">
+        <v>76</v>
+      </c>
+      <c r="F57" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>206</v>
+      </c>
+      <c r="B58" t="s">
+        <v>205</v>
+      </c>
+      <c r="C58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" t="s">
+        <v>2</v>
+      </c>
+      <c r="E58" t="s">
+        <v>77</v>
+      </c>
+      <c r="F58" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>206</v>
+      </c>
+      <c r="B59" t="s">
+        <v>205</v>
+      </c>
+      <c r="C59" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" t="s">
+        <v>2</v>
+      </c>
+      <c r="E59" t="s">
+        <v>78</v>
+      </c>
+      <c r="F59" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>206</v>
+      </c>
+      <c r="B60" t="s">
+        <v>205</v>
+      </c>
+      <c r="C60" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" t="s">
+        <v>2</v>
+      </c>
+      <c r="E60" t="s">
+        <v>79</v>
+      </c>
+      <c r="F60" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>206</v>
+      </c>
+      <c r="B61" t="s">
+        <v>205</v>
+      </c>
+      <c r="C61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" t="s">
+        <v>2</v>
+      </c>
+      <c r="E61" t="s">
+        <v>80</v>
+      </c>
+      <c r="F61" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>206</v>
+      </c>
+      <c r="B62" t="s">
+        <v>205</v>
+      </c>
+      <c r="C62" t="s">
+        <v>15</v>
+      </c>
+      <c r="D62" t="s">
+        <v>2</v>
+      </c>
+      <c r="E62" t="s">
+        <v>81</v>
+      </c>
+      <c r="F62" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>206</v>
+      </c>
+      <c r="B63" t="s">
+        <v>205</v>
+      </c>
+      <c r="C63" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" t="s">
+        <v>2</v>
+      </c>
+      <c r="E63" t="s">
+        <v>82</v>
+      </c>
+      <c r="F63" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>206</v>
+      </c>
+      <c r="B64" t="s">
+        <v>205</v>
+      </c>
+      <c r="C64" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" t="s">
+        <v>2</v>
+      </c>
+      <c r="E64" t="s">
+        <v>83</v>
+      </c>
+      <c r="F64" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>206</v>
+      </c>
+      <c r="B65" t="s">
+        <v>205</v>
+      </c>
+      <c r="C65" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" t="s">
+        <v>2</v>
+      </c>
+      <c r="E65" t="s">
+        <v>84</v>
+      </c>
+      <c r="F65" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>206</v>
+      </c>
+      <c r="B66" t="s">
+        <v>205</v>
+      </c>
+      <c r="C66" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" t="s">
+        <v>2</v>
+      </c>
+      <c r="E66" t="s">
+        <v>85</v>
+      </c>
+      <c r="F66" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>206</v>
+      </c>
+      <c r="B67" t="s">
+        <v>205</v>
+      </c>
+      <c r="C67" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" t="s">
+        <v>2</v>
+      </c>
+      <c r="E67" t="s">
+        <v>86</v>
+      </c>
+      <c r="F67" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>206</v>
+      </c>
+      <c r="B68" t="s">
+        <v>205</v>
+      </c>
+      <c r="C68" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68" t="s">
+        <v>2</v>
+      </c>
+      <c r="E68" t="s">
+        <v>87</v>
+      </c>
+      <c r="F68" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>206</v>
+      </c>
+      <c r="B69" t="s">
+        <v>205</v>
+      </c>
+      <c r="C69" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" t="s">
+        <v>2</v>
+      </c>
+      <c r="E69" t="s">
+        <v>88</v>
+      </c>
+      <c r="F69" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>206</v>
+      </c>
+      <c r="B70" t="s">
+        <v>205</v>
+      </c>
+      <c r="C70" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" t="s">
+        <v>2</v>
+      </c>
+      <c r="E70" t="s">
+        <v>89</v>
+      </c>
+      <c r="F70" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>206</v>
+      </c>
+      <c r="B71" t="s">
+        <v>205</v>
+      </c>
+      <c r="C71" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71" t="s">
+        <v>2</v>
+      </c>
+      <c r="E71" t="s">
         <v>90</v>
+      </c>
+      <c r="F71" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>206</v>
+      </c>
+      <c r="B72" t="s">
+        <v>205</v>
+      </c>
+      <c r="C72" t="s">
+        <v>15</v>
+      </c>
+      <c r="D72" t="s">
+        <v>2</v>
+      </c>
+      <c r="E72" t="s">
+        <v>91</v>
+      </c>
+      <c r="F72" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>206</v>
+      </c>
+      <c r="B73" t="s">
+        <v>205</v>
+      </c>
+      <c r="C73" t="s">
+        <v>15</v>
+      </c>
+      <c r="D73" t="s">
+        <v>2</v>
+      </c>
+      <c r="E73" t="s">
+        <v>92</v>
+      </c>
+      <c r="F73" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>206</v>
+      </c>
+      <c r="B74" t="s">
+        <v>205</v>
+      </c>
+      <c r="C74" t="s">
+        <v>15</v>
+      </c>
+      <c r="D74" t="s">
+        <v>2</v>
+      </c>
+      <c r="E74" t="s">
+        <v>93</v>
+      </c>
+      <c r="F74" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>206</v>
+      </c>
+      <c r="B75" t="s">
+        <v>205</v>
+      </c>
+      <c r="C75" t="s">
+        <v>15</v>
+      </c>
+      <c r="D75" t="s">
+        <v>2</v>
+      </c>
+      <c r="E75" t="s">
+        <v>94</v>
+      </c>
+      <c r="F75" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>206</v>
+      </c>
+      <c r="B76" t="s">
+        <v>205</v>
+      </c>
+      <c r="C76" t="s">
+        <v>15</v>
+      </c>
+      <c r="D76" t="s">
+        <v>2</v>
+      </c>
+      <c r="E76" t="s">
+        <v>95</v>
+      </c>
+      <c r="F76" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>206</v>
+      </c>
+      <c r="B77" t="s">
+        <v>205</v>
+      </c>
+      <c r="C77" t="s">
+        <v>15</v>
+      </c>
+      <c r="D77" t="s">
+        <v>2</v>
+      </c>
+      <c r="E77" t="s">
+        <v>96</v>
+      </c>
+      <c r="F77" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>206</v>
+      </c>
+      <c r="B78" t="s">
+        <v>205</v>
+      </c>
+      <c r="C78" t="s">
+        <v>15</v>
+      </c>
+      <c r="D78" t="s">
+        <v>2</v>
+      </c>
+      <c r="E78" t="s">
+        <v>97</v>
+      </c>
+      <c r="F78" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>206</v>
+      </c>
+      <c r="B79" t="s">
+        <v>205</v>
+      </c>
+      <c r="C79" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79" t="s">
+        <v>2</v>
+      </c>
+      <c r="E79" t="s">
+        <v>98</v>
+      </c>
+      <c r="F79" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>206</v>
+      </c>
+      <c r="B80" t="s">
+        <v>205</v>
+      </c>
+      <c r="C80" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80" t="s">
+        <v>2</v>
+      </c>
+      <c r="E80" t="s">
+        <v>99</v>
+      </c>
+      <c r="F80" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>206</v>
+      </c>
+      <c r="B81" t="s">
+        <v>205</v>
+      </c>
+      <c r="C81" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81" t="s">
+        <v>2</v>
+      </c>
+      <c r="E81" t="s">
+        <v>100</v>
+      </c>
+      <c r="F81" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>206</v>
+      </c>
+      <c r="B82" t="s">
+        <v>205</v>
+      </c>
+      <c r="C82" t="s">
+        <v>15</v>
+      </c>
+      <c r="D82" t="s">
+        <v>2</v>
+      </c>
+      <c r="E82" t="s">
+        <v>101</v>
+      </c>
+      <c r="F82" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>206</v>
+      </c>
+      <c r="B83" t="s">
+        <v>205</v>
+      </c>
+      <c r="C83" t="s">
+        <v>15</v>
+      </c>
+      <c r="D83" t="s">
+        <v>2</v>
+      </c>
+      <c r="E83" t="s">
+        <v>102</v>
+      </c>
+      <c r="F83" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>206</v>
+      </c>
+      <c r="B84" t="s">
+        <v>205</v>
+      </c>
+      <c r="C84" t="s">
+        <v>15</v>
+      </c>
+      <c r="D84" t="s">
+        <v>2</v>
+      </c>
+      <c r="E84" t="s">
+        <v>103</v>
+      </c>
+      <c r="F84" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>210</v>
+      </c>
+      <c r="B85" t="s">
+        <v>209</v>
+      </c>
+      <c r="C85" t="s">
+        <v>15</v>
+      </c>
+      <c r="D85" t="s">
+        <v>3</v>
+      </c>
+      <c r="E85" t="s">
+        <v>104</v>
+      </c>
+      <c r="F85" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>210</v>
+      </c>
+      <c r="B86" t="s">
+        <v>209</v>
+      </c>
+      <c r="C86" t="s">
+        <v>15</v>
+      </c>
+      <c r="D86" t="s">
+        <v>3</v>
+      </c>
+      <c r="E86" t="s">
+        <v>105</v>
+      </c>
+      <c r="F86" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>208</v>
+      </c>
+      <c r="B87" t="s">
+        <v>207</v>
+      </c>
+      <c r="C87" t="s">
+        <v>15</v>
+      </c>
+      <c r="D87" t="s">
+        <v>4</v>
+      </c>
+      <c r="E87" t="s">
+        <v>106</v>
+      </c>
+      <c r="F87" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>208</v>
+      </c>
+      <c r="B88" t="s">
+        <v>207</v>
+      </c>
+      <c r="C88" t="s">
+        <v>15</v>
+      </c>
+      <c r="D88" t="s">
+        <v>4</v>
+      </c>
+      <c r="E88" t="s">
+        <v>107</v>
+      </c>
+      <c r="F88" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>208</v>
+      </c>
+      <c r="B89" t="s">
+        <v>207</v>
+      </c>
+      <c r="C89" t="s">
+        <v>15</v>
+      </c>
+      <c r="D89" t="s">
+        <v>4</v>
+      </c>
+      <c r="E89" t="s">
+        <v>108</v>
+      </c>
+      <c r="F89" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>208</v>
+      </c>
+      <c r="B90" t="s">
+        <v>207</v>
+      </c>
+      <c r="C90" t="s">
+        <v>15</v>
+      </c>
+      <c r="D90" t="s">
+        <v>4</v>
+      </c>
+      <c r="E90" t="s">
+        <v>109</v>
+      </c>
+      <c r="F90" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>208</v>
+      </c>
+      <c r="B91" t="s">
+        <v>207</v>
+      </c>
+      <c r="C91" t="s">
+        <v>15</v>
+      </c>
+      <c r="D91" t="s">
+        <v>4</v>
+      </c>
+      <c r="E91" t="s">
+        <v>110</v>
+      </c>
+      <c r="F91" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>208</v>
+      </c>
+      <c r="B92" t="s">
+        <v>207</v>
+      </c>
+      <c r="C92" t="s">
+        <v>15</v>
+      </c>
+      <c r="D92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E92" t="s">
+        <v>111</v>
+      </c>
+      <c r="F92" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>208</v>
+      </c>
+      <c r="B93" t="s">
+        <v>207</v>
+      </c>
+      <c r="C93" t="s">
+        <v>15</v>
+      </c>
+      <c r="D93" t="s">
+        <v>4</v>
+      </c>
+      <c r="E93" t="s">
+        <v>112</v>
+      </c>
+      <c r="F93" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>